<commit_message>
Completed Task1 (Simple Sequence Analysis).
</commit_message>
<xml_diff>
--- a/Translation.xlsx
+++ b/Translation.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="277" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="278" uniqueCount="42">
   <si>
     <t xml:space="preserve">Transcription and Translation Exercise</t>
   </si>
@@ -143,7 +143,10 @@
     </r>
   </si>
   <si>
-    <t xml:space="preserve">(Tyr)</t>
+    <t xml:space="preserve">Met</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Begynner på Met!!</t>
   </si>
   <si>
     <r>
@@ -192,7 +195,7 @@
     </r>
   </si>
   <si>
-    <t xml:space="preserve">STOP</t>
+    <t xml:space="preserve">Ser</t>
   </si>
   <si>
     <r>
@@ -218,7 +221,7 @@
     </r>
   </si>
   <si>
-    <t xml:space="preserve">Ala</t>
+    <t xml:space="preserve">Gly</t>
   </si>
   <si>
     <r>
@@ -244,19 +247,19 @@
     </r>
   </si>
   <si>
-    <t xml:space="preserve">Val</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Gln</t>
+    <t xml:space="preserve">His</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Leu</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Pro</t>
   </si>
   <si>
     <t xml:space="preserve">Arg</t>
   </si>
   <si>
-    <t xml:space="preserve">Pro</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Ser</t>
+    <t xml:space="preserve">Thr</t>
   </si>
   <si>
     <r>
@@ -311,16 +314,19 @@
     <t xml:space="preserve">Gene/template</t>
   </si>
   <si>
-    <t xml:space="preserve">Gly</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Cys</t>
-  </si>
-  <si>
-    <t xml:space="preserve">His</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Thr</t>
+    <t xml:space="preserve">Tyr</t>
+  </si>
+  <si>
+    <t xml:space="preserve">STOP</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ala</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Val</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Gln</t>
   </si>
 </sst>
 </file>
@@ -651,10 +657,10 @@
   <dimension ref="A1:M33"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E10" activeCellId="0" sqref="E10"/>
+      <selection pane="topLeft" activeCell="G11" activeCellId="0" sqref="G11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.15234375" defaultRowHeight="18.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="9.16015625" defaultRowHeight="18.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="9.14"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="10.85"/>
@@ -719,7 +725,7 @@
       <c r="J4" s="10"/>
       <c r="K4" s="10"/>
     </row>
-    <row r="5" customFormat="false" ht="19.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="5" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="15" t="s">
         <v>13</v>
       </c>
@@ -767,7 +773,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="8" customFormat="false" ht="19.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="8" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="15" t="s">
         <v>14</v>
       </c>
@@ -816,8 +822,11 @@
       <c r="E10" s="14" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="11" customFormat="false" ht="23.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="F10" s="0" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="11" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="15" t="s">
         <v>13</v>
       </c>
@@ -828,7 +837,7 @@
         <v>13</v>
       </c>
       <c r="D11" s="16" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="E11" s="14"/>
     </row>
@@ -843,7 +852,7 @@
         <v>16</v>
       </c>
       <c r="D12" s="16" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="E12" s="14"/>
     </row>
@@ -861,10 +870,10 @@
         <v>13</v>
       </c>
       <c r="E13" s="14" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="14" customFormat="false" ht="23.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="14" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="15" t="s">
         <v>15</v>
       </c>
@@ -875,7 +884,7 @@
         <v>15</v>
       </c>
       <c r="D14" s="16" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="E14" s="14"/>
     </row>
@@ -908,7 +917,7 @@
         <v>10</v>
       </c>
       <c r="E16" s="14" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -937,7 +946,7 @@
         <v>10</v>
       </c>
       <c r="D18" s="16" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="E18" s="14"/>
     </row>
@@ -955,10 +964,10 @@
         <v>16</v>
       </c>
       <c r="E19" s="14" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="20" customFormat="false" ht="23.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="20" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="15" t="s">
         <v>10</v>
       </c>
@@ -984,7 +993,7 @@
         <v>10</v>
       </c>
       <c r="D21" s="16" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="E21" s="14"/>
     </row>
@@ -1002,7 +1011,7 @@
         <v>15</v>
       </c>
       <c r="E22" s="14" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1016,7 +1025,7 @@
         <v>13</v>
       </c>
       <c r="D23" s="16" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="E23" s="14"/>
     </row>
@@ -1031,7 +1040,7 @@
         <v>10</v>
       </c>
       <c r="D24" s="16" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="E24" s="14"/>
     </row>
@@ -1049,7 +1058,7 @@
         <v>13</v>
       </c>
       <c r="E25" s="14" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1063,7 +1072,7 @@
         <v>13</v>
       </c>
       <c r="D26" s="16" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="E26" s="14"/>
     </row>
@@ -1078,7 +1087,7 @@
         <v>10</v>
       </c>
       <c r="D27" s="16" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="E27" s="14"/>
     </row>
@@ -1096,7 +1105,7 @@
         <v>10</v>
       </c>
       <c r="E28" s="14" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1110,7 +1119,7 @@
         <v>13</v>
       </c>
       <c r="D29" s="16" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="E29" s="14"/>
     </row>
@@ -1143,30 +1152,30 @@
         <v>13</v>
       </c>
       <c r="E31" s="14" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="17" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="B32" s="18" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="C32" s="18" t="s">
         <v>19</v>
       </c>
       <c r="D32" s="19" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="E32" s="18"/>
     </row>
     <row r="33" customFormat="false" ht="38.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="15" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="B33" s="14" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="C33" s="14"/>
       <c r="D33" s="14"/>
@@ -1194,10 +1203,10 @@
   <dimension ref="A1:M33"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F20" activeCellId="0" sqref="F20"/>
+      <selection pane="topLeft" activeCell="F10" activeCellId="0" sqref="F10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.15234375" defaultRowHeight="18.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="9.16015625" defaultRowHeight="18.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="9.14"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="10.85"/>
@@ -1275,9 +1284,7 @@
       <c r="D5" s="16" t="s">
         <v>13</v>
       </c>
-      <c r="E5" s="14" t="s">
-        <v>36</v>
-      </c>
+      <c r="E5" s="14"/>
     </row>
     <row r="6" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="15" t="s">
@@ -1307,7 +1314,9 @@
       <c r="D7" s="16" t="s">
         <v>10</v>
       </c>
-      <c r="E7" s="14"/>
+      <c r="E7" s="14" t="s">
+        <v>31</v>
+      </c>
     </row>
     <row r="8" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="15" t="s">
@@ -1322,9 +1331,7 @@
       <c r="D8" s="16" t="s">
         <v>16</v>
       </c>
-      <c r="E8" s="14" t="s">
-        <v>30</v>
-      </c>
+      <c r="E8" s="14"/>
       <c r="H8" s="0" t="s">
         <v>17</v>
       </c>
@@ -1360,7 +1367,9 @@
       <c r="D10" s="16" t="s">
         <v>16</v>
       </c>
-      <c r="E10" s="14"/>
+      <c r="E10" s="14" t="s">
+        <v>37</v>
+      </c>
     </row>
     <row r="11" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="15" t="s">
@@ -1375,9 +1384,7 @@
       <c r="D11" s="16" t="s">
         <v>13</v>
       </c>
-      <c r="E11" s="14" t="s">
-        <v>37</v>
-      </c>
+      <c r="E11" s="14"/>
     </row>
     <row r="12" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="15" t="s">
@@ -1407,7 +1414,9 @@
       <c r="D13" s="16" t="s">
         <v>10</v>
       </c>
-      <c r="E13" s="14"/>
+      <c r="E13" s="14" t="s">
+        <v>38</v>
+      </c>
     </row>
     <row r="14" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="15" t="s">
@@ -1422,9 +1431,7 @@
       <c r="D14" s="16" t="s">
         <v>15</v>
       </c>
-      <c r="E14" s="14" t="s">
-        <v>38</v>
-      </c>
+      <c r="E14" s="14"/>
     </row>
     <row r="15" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="15" t="s">
@@ -1454,7 +1461,9 @@
       <c r="D16" s="16" t="s">
         <v>13</v>
       </c>
-      <c r="E16" s="14"/>
+      <c r="E16" s="14" t="s">
+        <v>39</v>
+      </c>
     </row>
     <row r="17" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="15" t="s">
@@ -1469,9 +1478,7 @@
       <c r="D17" s="16" t="s">
         <v>10</v>
       </c>
-      <c r="E17" s="14" t="s">
-        <v>31</v>
-      </c>
+      <c r="E17" s="14"/>
     </row>
     <row r="18" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="15" t="s">
@@ -1501,7 +1508,9 @@
       <c r="D19" s="16" t="s">
         <v>15</v>
       </c>
-      <c r="E19" s="14"/>
+      <c r="E19" s="14" t="s">
+        <v>40</v>
+      </c>
     </row>
     <row r="20" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="15" t="s">
@@ -1516,9 +1525,7 @@
       <c r="D20" s="16" t="s">
         <v>10</v>
       </c>
-      <c r="E20" s="14" t="s">
-        <v>39</v>
-      </c>
+      <c r="E20" s="14"/>
     </row>
     <row r="21" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="15" t="s">
@@ -1548,7 +1555,9 @@
       <c r="D22" s="16" t="s">
         <v>16</v>
       </c>
-      <c r="E22" s="14"/>
+      <c r="E22" s="14" t="s">
+        <v>41</v>
+      </c>
     </row>
     <row r="23" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="15" t="s">
@@ -1563,9 +1572,7 @@
       <c r="D23" s="16" t="s">
         <v>13</v>
       </c>
-      <c r="E23" s="14" t="s">
-        <v>37</v>
-      </c>
+      <c r="E23" s="14"/>
     </row>
     <row r="24" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="15" t="s">
@@ -1595,7 +1602,9 @@
       <c r="D25" s="16" t="s">
         <v>10</v>
       </c>
-      <c r="E25" s="14"/>
+      <c r="E25" s="14" t="s">
+        <v>31</v>
+      </c>
     </row>
     <row r="26" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="15" t="s">
@@ -1610,9 +1619,7 @@
       <c r="D26" s="16" t="s">
         <v>13</v>
       </c>
-      <c r="E26" s="14" t="s">
-        <v>29</v>
-      </c>
+      <c r="E26" s="14"/>
     </row>
     <row r="27" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="15" t="s">
@@ -1642,7 +1649,9 @@
       <c r="D28" s="16" t="s">
         <v>13</v>
       </c>
-      <c r="E28" s="14"/>
+      <c r="E28" s="14" t="s">
+        <v>30</v>
+      </c>
     </row>
     <row r="29" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="15" t="s">
@@ -1657,9 +1666,7 @@
       <c r="D29" s="16" t="s">
         <v>13</v>
       </c>
-      <c r="E29" s="14" t="s">
-        <v>23</v>
-      </c>
+      <c r="E29" s="14"/>
     </row>
     <row r="30" customFormat="false" ht="23.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="15" t="s">
@@ -1672,7 +1679,7 @@
         <v>14</v>
       </c>
       <c r="D30" s="16" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="E30" s="14"/>
     </row>
@@ -1689,17 +1696,19 @@
       <c r="D31" s="16" t="s">
         <v>10</v>
       </c>
-      <c r="E31" s="14"/>
+      <c r="E31" s="14" t="s">
+        <v>24</v>
+      </c>
     </row>
     <row r="32" customFormat="false" ht="22.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="17" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="B32" s="18" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="C32" s="18" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="D32" s="19" t="s">
         <v>19</v>
@@ -1708,10 +1717,10 @@
     </row>
     <row r="33" customFormat="false" ht="57" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="14" t="s">
+        <v>36</v>
+      </c>
+      <c r="B33" s="15" t="s">
         <v>35</v>
-      </c>
-      <c r="B33" s="15" t="s">
-        <v>34</v>
       </c>
       <c r="C33" s="14"/>
       <c r="D33" s="14"/>

</xml_diff>